<commit_message>
Fix donwload upload format
</commit_message>
<xml_diff>
--- a/storage/app/upload_format/JORequestForm.xlsx
+++ b/storage/app/upload_format/JORequestForm.xlsx
@@ -416,15 +416,147 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -437,9 +569,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -448,135 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,7 +615,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -918,8 +918,8 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,14 +953,14 @@
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -968,14 +968,14 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="7"/>
@@ -983,14 +983,14 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="7"/>
@@ -998,179 +998,179 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="61"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="64"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="67" t="s">
+      <c r="I8" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="68"/>
-      <c r="K8" s="69"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="72"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="67" t="s">
+      <c r="I9" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="68"/>
-      <c r="K9" s="69"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="75"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="76"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="78"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
     </row>
     <row r="11" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="82"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="55"/>
     </row>
     <row r="12" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="48"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
     </row>
     <row r="13" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="53"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="75"/>
       <c r="L13" s="22"/>
     </row>
     <row r="14" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="45"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="64"/>
     </row>
     <row r="15" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="72"/>
       <c r="G15" s="13" t="s">
         <v>17</v>
       </c>
@@ -1183,55 +1183,55 @@
     </row>
     <row r="16" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="50"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>
       <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="50"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="19"/>
       <c r="H17" s="18"/>
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
       <c r="G18" s="19"/>
       <c r="H18" s="18"/>
       <c r="I18" s="17"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
       <c r="G19" s="15"/>
       <c r="H19" s="16"/>
       <c r="I19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="82"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="17"/>
@@ -1254,13 +1254,13 @@
       <c r="D22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="42"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="72"/>
       <c r="J22" s="13" t="s">
         <v>23</v>
       </c>
@@ -1273,11 +1273,11 @@
       <c r="B23" s="18"/>
       <c r="C23" s="26"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="31"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
       <c r="J23" s="18"/>
       <c r="K23" s="28" t="s">
         <v>27</v>
@@ -1288,11 +1288,11 @@
       <c r="B24" s="19"/>
       <c r="C24" s="17"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="69"/>
       <c r="J24" s="18"/>
       <c r="K24" s="28" t="s">
         <v>27</v>
@@ -1303,11 +1303,11 @@
       <c r="B25" s="19"/>
       <c r="C25" s="17"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="31"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="69"/>
       <c r="J25" s="18"/>
       <c r="K25" s="28" t="s">
         <v>27</v>
@@ -1318,11 +1318,11 @@
       <c r="B26" s="15"/>
       <c r="C26" s="27"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="31"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="69"/>
       <c r="J26" s="16"/>
       <c r="K26" s="28" t="s">
         <v>27</v>
@@ -1332,19 +1332,37 @@
       <c r="A27" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="34"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="I7:K7"/>
@@ -1360,25 +1378,7 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:K11"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
     <mergeCell ref="B14:K14"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>